<commit_message>
Adicionado o gráfico de burndown
</commit_message>
<xml_diff>
--- a/Documentação/Gestão/Product BackLog StrawTech.xlsx
+++ b/Documentação/Gestão/Product BackLog StrawTech.xlsx
@@ -8,19 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SPTECHOISAS\sprint2\Sprint2\Documentação\Gestão\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8EA6D5-EC5A-41BA-9267-DC33ECD38704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F802E071-1661-4274-AB15-43EDCB62EF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="129">
   <si>
     <t>Product BACKLOG</t>
   </si>
@@ -62,9 +78,6 @@
   </si>
   <si>
     <t>Calculadora financeira</t>
-  </si>
-  <si>
-    <t>Desenvolver uma calculadora que aoresenta o projeto conforme a pesquisa</t>
   </si>
   <si>
     <t>Grande</t>
@@ -387,12 +400,36 @@
   <si>
     <t>Utilizar o chart js para alterar o design dos gráficos na tela do site</t>
   </si>
+  <si>
+    <t>Desenvolver uma calculadora que apresenta o projeto conforme a pesquisa</t>
+  </si>
+  <si>
+    <t>SP1</t>
+  </si>
+  <si>
+    <t>SP2 - B</t>
+  </si>
+  <si>
+    <t>SP2 - C</t>
+  </si>
+  <si>
+    <t>SP2 - D</t>
+  </si>
+  <si>
+    <t>SP2 - A</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>TABELA - GRÁFICO DE BURNDOWN</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -438,6 +475,20 @@
     <font>
       <b/>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -573,7 +624,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -639,6 +690,15 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,6 +714,1019 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
+                <a:gradFill>
+                  <a:gsLst>
+                    <a:gs pos="0">
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                    <a:gs pos="100000">
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="85000"/>
+                        <a:lumOff val="15000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                  </a:gsLst>
+                  <a:lin ang="5400000" scaled="0"/>
+                </a:gradFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Gráfico de Burndown</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="85000"/>
+                      <a:lumOff val="15000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Página1!$J$6:$O$6</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SP1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SP2 - A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SP2 - B</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SP2 - C</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>SP2 - D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Página1!$J$7:$O$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>598</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>382</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-69F6-479F-BEB5-688D23F5E779}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1407992736"/>
+        <c:axId val="750245664"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1407992736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="750245664"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="750245664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1407992736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="234">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr/>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9575">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="17"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1440" b="0" kern="1200" cap="all" spc="0" baseline="0">
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>273424</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>17930</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>497541</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>340659</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B918241D-B542-EBAB-0728-F2EFAE0DC165}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Planilha1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="7">
+          <cell r="I7" t="str">
+            <v>TOTAL</v>
+          </cell>
+          <cell r="J7" t="str">
+            <v>SP1</v>
+          </cell>
+          <cell r="K7" t="str">
+            <v>SP2 - A</v>
+          </cell>
+          <cell r="L7" t="str">
+            <v xml:space="preserve">SP2 - B </v>
+          </cell>
+          <cell r="M7" t="str">
+            <v>2P2 - C</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="I8">
+            <v>472</v>
+          </cell>
+          <cell r="J8">
+            <v>254</v>
+          </cell>
+          <cell r="K8">
+            <v>178</v>
+          </cell>
+          <cell r="L8">
+            <v>94</v>
+          </cell>
+          <cell r="M8">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -859,8 +1932,8 @@
   </sheetPr>
   <dimension ref="A1:Z957"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -868,6 +1941,8 @@
     <col min="1" max="1" width="18.109375" customWidth="1"/>
     <col min="2" max="2" width="46.21875" customWidth="1"/>
     <col min="3" max="3" width="86.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
     <col min="8" max="8" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1019,13 +2094,13 @@
         <v>13</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>14</v>
+        <v>121</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="8">
         <v>21</v>
@@ -1037,12 +2112,14 @@
         <v>12</v>
       </c>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
+      <c r="J5" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
@@ -1058,10 +2135,10 @@
     <row r="6" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>17</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>10</v>
@@ -1079,12 +2156,24 @@
         <v>12</v>
       </c>
       <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
+      <c r="J6" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="K6" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="L6" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="M6" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="N6" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="O6" s="23" t="s">
+        <v>125</v>
+      </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
@@ -1100,13 +2189,13 @@
     <row r="7" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>11</v>
@@ -1121,12 +2210,24 @@
         <v>12</v>
       </c>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
+      <c r="J7" s="23">
+        <v>598</v>
+      </c>
+      <c r="K7" s="23">
+        <v>382</v>
+      </c>
+      <c r="L7" s="23">
+        <v>215</v>
+      </c>
+      <c r="M7" s="23">
+        <v>88</v>
+      </c>
+      <c r="N7" s="23">
+        <v>49</v>
+      </c>
+      <c r="O7" s="23">
+        <v>0</v>
+      </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
@@ -1142,10 +2243,10 @@
     <row r="8" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>10</v>
@@ -1170,7 +2271,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
+      <c r="Q8" s="24"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
@@ -1184,16 +2285,16 @@
     <row r="9" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" s="8">
         <v>21</v>
@@ -1226,10 +2327,10 @@
     <row r="10" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>10</v>
@@ -1268,10 +2369,10 @@
     <row r="11" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>27</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>10</v>
@@ -1310,16 +2411,16 @@
     <row r="12" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="8">
         <v>13</v>
@@ -1352,16 +2453,16 @@
     <row r="13" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F13" s="8">
         <v>21</v>
@@ -1394,16 +2495,16 @@
     <row r="14" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" s="8">
         <v>21</v>
@@ -1436,16 +2537,16 @@
     <row r="15" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F15" s="8">
         <v>8</v>
@@ -1478,16 +2579,16 @@
     <row r="16" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F16" s="8">
         <v>8</v>
@@ -1520,16 +2621,16 @@
     <row r="17" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F17" s="8">
         <v>21</v>
@@ -1562,13 +2663,13 @@
     <row r="18" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="D18" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>11</v>
@@ -1604,16 +2705,16 @@
     <row r="19" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>45</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F19" s="8">
         <v>13</v>
@@ -1646,16 +2747,16 @@
     <row r="20" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F20" s="8">
         <v>13</v>
@@ -1688,16 +2789,16 @@
     <row r="21" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F21" s="8">
         <v>21</v>
@@ -1758,21 +2859,25 @@
     <row r="23" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="F23" s="5">
+        <v>21</v>
+      </c>
+      <c r="G23" s="5">
+        <v>1</v>
+      </c>
       <c r="H23" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1796,21 +2901,25 @@
     <row r="24" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>54</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="F24" s="5">
+        <v>21</v>
+      </c>
+      <c r="G24" s="5">
+        <v>1</v>
+      </c>
       <c r="H24" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1834,21 +2943,25 @@
     <row r="25" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="F25" s="5">
+        <v>21</v>
+      </c>
+      <c r="G25" s="5">
+        <v>1</v>
+      </c>
       <c r="H25" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -1872,21 +2985,25 @@
     <row r="26" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="F26" s="5">
+        <v>21</v>
+      </c>
+      <c r="G26" s="5">
+        <v>1</v>
+      </c>
       <c r="H26" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1910,21 +3027,25 @@
     <row r="27" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="F27" s="5">
+        <v>21</v>
+      </c>
+      <c r="G27" s="5">
+        <v>1</v>
+      </c>
       <c r="H27" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -1948,21 +3069,25 @@
     <row r="28" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>62</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F28" s="5">
+        <v>13</v>
+      </c>
+      <c r="G28" s="5">
+        <v>2</v>
+      </c>
       <c r="H28" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -1986,21 +3111,25 @@
     <row r="29" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F29" s="5">
+        <v>13</v>
+      </c>
+      <c r="G29" s="5">
+        <v>1</v>
+      </c>
       <c r="H29" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -2024,21 +3153,25 @@
     <row r="30" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>65</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>66</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F30" s="5">
+        <v>13</v>
+      </c>
+      <c r="G30" s="5">
+        <v>1</v>
+      </c>
       <c r="H30" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -2062,21 +3195,25 @@
     <row r="31" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>68</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F31" s="5">
+        <v>8</v>
+      </c>
+      <c r="G31" s="5">
+        <v>3</v>
+      </c>
       <c r="H31" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -2100,10 +3237,10 @@
     <row r="32" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>70</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>10</v>
@@ -2111,10 +3248,14 @@
       <c r="E32" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
+      <c r="F32" s="5">
+        <v>5</v>
+      </c>
+      <c r="G32" s="5">
+        <v>1</v>
+      </c>
       <c r="H32" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -2138,10 +3279,10 @@
     <row r="33" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>72</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>10</v>
@@ -2149,10 +3290,14 @@
       <c r="E33" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
+      <c r="F33" s="5">
+        <v>5</v>
+      </c>
+      <c r="G33" s="5">
+        <v>1</v>
+      </c>
       <c r="H33" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -2176,10 +3321,10 @@
     <row r="34" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>74</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>10</v>
@@ -2187,10 +3332,14 @@
       <c r="E34" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
+      <c r="F34" s="5">
+        <v>5</v>
+      </c>
+      <c r="G34" s="5">
+        <v>3</v>
+      </c>
       <c r="H34" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -2242,21 +3391,25 @@
     <row r="36" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="D36" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="5">
+        <v>21</v>
+      </c>
+      <c r="G36" s="5">
+        <v>2</v>
+      </c>
+      <c r="H36" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="9" t="s">
-        <v>77</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
@@ -2280,21 +3433,25 @@
     <row r="37" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C37" s="9" t="s">
-        <v>79</v>
-      </c>
       <c r="D37" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E37" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
+      <c r="F37" s="5">
+        <v>5</v>
+      </c>
+      <c r="G37" s="5">
+        <v>3</v>
+      </c>
       <c r="H37" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
@@ -2318,21 +3475,25 @@
     <row r="38" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>81</v>
-      </c>
       <c r="D38" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
+      <c r="F38" s="5">
+        <v>5</v>
+      </c>
+      <c r="G38" s="5">
+        <v>3</v>
+      </c>
       <c r="H38" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -2356,21 +3517,25 @@
     <row r="39" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>83</v>
-      </c>
       <c r="D39" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F39" s="5">
+        <v>8</v>
+      </c>
+      <c r="G39" s="5">
+        <v>2</v>
+      </c>
       <c r="H39" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -2394,21 +3559,25 @@
     <row r="40" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>85</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="F40" s="5">
+        <v>21</v>
+      </c>
+      <c r="G40" s="5">
+        <v>1</v>
+      </c>
       <c r="H40" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -2432,21 +3601,25 @@
     <row r="41" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C41" s="9" t="s">
-        <v>87</v>
-      </c>
       <c r="D41" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E41" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
+      <c r="F41" s="5">
+        <v>5</v>
+      </c>
+      <c r="G41" s="5">
+        <v>3</v>
+      </c>
       <c r="H41" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
@@ -2470,21 +3643,25 @@
     <row r="42" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C42" s="9" t="s">
-        <v>89</v>
-      </c>
       <c r="D42" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E42" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
+      <c r="F42" s="5">
+        <v>5</v>
+      </c>
+      <c r="G42" s="5">
+        <v>3</v>
+      </c>
       <c r="H42" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -2508,21 +3685,25 @@
     <row r="43" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C43" s="9" t="s">
-        <v>91</v>
-      </c>
       <c r="D43" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E43" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
+      <c r="F43" s="5">
+        <v>5</v>
+      </c>
+      <c r="G43" s="5">
+        <v>3</v>
+      </c>
       <c r="H43" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -2546,21 +3727,25 @@
     <row r="44" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>93</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F44" s="5">
+        <v>13</v>
+      </c>
+      <c r="G44" s="5">
+        <v>1</v>
+      </c>
       <c r="H44" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -2584,21 +3769,25 @@
     <row r="45" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>94</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>95</v>
       </c>
       <c r="D45" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F45" s="5">
+        <v>13</v>
+      </c>
+      <c r="G45" s="5">
+        <v>1</v>
+      </c>
       <c r="H45" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -2622,21 +3811,25 @@
     <row r="46" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="9" t="s">
         <v>96</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>97</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F46" s="5">
+        <v>13</v>
+      </c>
+      <c r="G46" s="5">
+        <v>1</v>
+      </c>
       <c r="H46" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
@@ -2660,20 +3853,26 @@
     <row r="47" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="D47" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F47" s="6"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F47" s="6">
+        <v>13</v>
+      </c>
+      <c r="G47" s="5">
+        <v>1</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
@@ -2724,10 +3923,10 @@
     <row r="49" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>100</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>101</v>
       </c>
       <c r="D49" s="10" t="s">
         <v>10</v>
@@ -2735,10 +3934,14 @@
       <c r="E49" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
+      <c r="F49" s="5">
+        <v>5</v>
+      </c>
+      <c r="G49" s="5">
+        <v>2</v>
+      </c>
       <c r="H49" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
@@ -2762,21 +3965,25 @@
     <row r="50" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="D50" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F50" s="5">
+        <v>8</v>
+      </c>
+      <c r="G50" s="5">
+        <v>1</v>
+      </c>
       <c r="H50" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
@@ -2800,21 +4007,25 @@
     <row r="51" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>106</v>
       </c>
       <c r="D51" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F51" s="5">
+        <v>13</v>
+      </c>
+      <c r="G51" s="5">
+        <v>1</v>
+      </c>
       <c r="H51" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
@@ -2838,21 +4049,25 @@
     <row r="52" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="15"/>
       <c r="B52" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C52" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C52" s="6" t="s">
-        <v>108</v>
-      </c>
       <c r="D52" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
+        <v>29</v>
+      </c>
+      <c r="F52" s="6">
+        <v>13</v>
+      </c>
+      <c r="G52" s="6">
+        <v>1</v>
+      </c>
       <c r="H52" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -2904,10 +4119,10 @@
     <row r="54" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="9" t="s">
         <v>111</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>112</v>
       </c>
       <c r="D54" s="10" t="s">
         <v>10</v>
@@ -2915,10 +4130,14 @@
       <c r="E54" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
+      <c r="F54" s="5">
+        <v>5</v>
+      </c>
+      <c r="G54" s="5">
+        <v>3</v>
+      </c>
       <c r="H54" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
@@ -2942,10 +4161,10 @@
     <row r="55" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16"/>
       <c r="B55" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C55" s="17" t="s">
         <v>109</v>
-      </c>
-      <c r="C55" s="17" t="s">
-        <v>110</v>
       </c>
       <c r="D55" s="18" t="s">
         <v>10</v>
@@ -2953,10 +4172,14 @@
       <c r="E55" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
+      <c r="F55" s="17">
+        <v>5</v>
+      </c>
+      <c r="G55" s="17">
+        <v>3</v>
+      </c>
       <c r="H55" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
@@ -2980,10 +4203,10 @@
     <row r="56" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>10</v>
@@ -2991,10 +4214,14 @@
       <c r="E56" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
+      <c r="F56" s="3">
+        <v>5</v>
+      </c>
+      <c r="G56" s="3">
+        <v>3</v>
+      </c>
       <c r="H56" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
@@ -3018,21 +4245,25 @@
     <row r="57" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="F57" s="3">
+        <v>8</v>
+      </c>
+      <c r="G57" s="3">
+        <v>3</v>
+      </c>
       <c r="H57" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
@@ -3056,21 +4287,25 @@
     <row r="58" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>120</v>
-      </c>
       <c r="D58" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
+      <c r="F58" s="3">
+        <v>5</v>
+      </c>
+      <c r="G58" s="3">
+        <v>3</v>
+      </c>
       <c r="H58" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
@@ -3094,21 +4329,25 @@
     <row r="59" spans="1:26" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="F59" s="3">
+        <v>21</v>
+      </c>
+      <c r="G59" s="3">
+        <v>2</v>
+      </c>
       <c r="H59" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
@@ -28274,7 +29513,11 @@
       <c r="Z957" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J5:O5"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>